<commit_message>
Actaulizacion de carpeta fuera de C:
</commit_message>
<xml_diff>
--- a/Gantt Projecto.xlsx
+++ b/Gantt Projecto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a48e2bcde33f5/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7a48e2bcde33f5/Documents/Universidad/IC Desing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_B14AD35950FDCCBF891C87D97A696DC161B48F56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91772C22-03C3-4CF4-B818-116837A7E14A}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_B14AD35950FDCCBF891C87D97A696DC161B48F56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1B0A864-A026-49F2-9E12-BBB82C8FB5BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Tareas / Semana</t>
-  </si>
-  <si>
-    <t>Semana 18</t>
-  </si>
-  <si>
-    <t>Semana 19</t>
-  </si>
-  <si>
-    <t>Semana 20</t>
-  </si>
-  <si>
-    <t>Semana 21</t>
   </si>
   <si>
     <t>Semana 22</t>
@@ -259,15 +247,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC903E2B-9131-4042-BDB9-46624D405B9D}" name="Tabla1" displayName="Tabla1" ref="A1:S6" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:S6" xr:uid="{DC903E2B-9131-4042-BDB9-46624D405B9D}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC903E2B-9131-4042-BDB9-46624D405B9D}" name="Tabla1" displayName="Tabla1" ref="A1:O6" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:O6" xr:uid="{DC903E2B-9131-4042-BDB9-46624D405B9D}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{88D64E66-119D-44EF-AB72-C1E2EE4CF73F}" name="Tareas / Semana"/>
-    <tableColumn id="2" xr3:uid="{6FB7D8C9-666C-4D81-B665-F57761650324}" name="Semana 18"/>
-    <tableColumn id="3" xr3:uid="{62F728AA-3BEF-4526-BB17-2EDF7942A6C7}" name="Semana 19"/>
-    <tableColumn id="4" xr3:uid="{27412881-871A-4102-9532-BBA9D59DCF6F}" name="Semana 20"/>
-    <tableColumn id="5" xr3:uid="{04DE3845-9531-43C8-AD40-27C9D2C8537A}" name="Semana 21"/>
     <tableColumn id="6" xr3:uid="{4A52E6D3-73A5-4B5D-BB9F-6E2A51E7E85E}" name="Semana 22"/>
     <tableColumn id="7" xr3:uid="{A9FD674E-7835-45C2-B2F7-773695878E61}" name="Semana 23"/>
     <tableColumn id="8" xr3:uid="{85B32553-9DCC-466E-AEC1-061FB329F43A}" name="Semana 24"/>
@@ -574,15 +562,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,87 +616,75 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>